<commit_message>
done with lat long depth plots
</commit_message>
<xml_diff>
--- a/data/atl_ranges.xlsx
+++ b/data/atl_ranges.xlsx
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K717"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A343" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G352" sqref="G352"/>
+    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H348" sqref="H348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9527,13 +9527,13 @@
         <v>25</v>
       </c>
       <c r="E417" s="3">
-        <v>156.36260899999999</v>
+        <v>175.847984</v>
       </c>
       <c r="F417" s="3">
         <v>978048705219</v>
       </c>
       <c r="I417">
-        <f t="shared" ref="I417:I419" si="2">G417+H417</f>
+        <f t="shared" ref="I417:I418" si="2">G417+H417</f>
         <v>0</v>
       </c>
     </row>
@@ -9551,7 +9551,7 @@
         <v>25</v>
       </c>
       <c r="E418" s="3">
-        <v>156.36260899999999</v>
+        <v>175.847984</v>
       </c>
       <c r="F418" s="3">
         <v>1956107336960</v>
@@ -9575,7 +9575,7 @@
         <v>25</v>
       </c>
       <c r="E419" s="3">
-        <v>156.36260899999999</v>
+        <v>175.847984</v>
       </c>
       <c r="F419" s="3">
         <v>1538401.8555960001</v>
@@ -10688,6 +10688,12 @@
       <c r="D468" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E468" s="3">
+        <v>0</v>
+      </c>
+      <c r="F468" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A469" s="3" t="s">
@@ -10702,6 +10708,12 @@
       <c r="D469" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E469" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F469" s="5">
+        <v>627918300000000</v>
+      </c>
     </row>
     <row r="470" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A470" s="3" t="s">
@@ -10716,6 +10728,12 @@
       <c r="D470" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E470" s="3">
+        <v>5</v>
+      </c>
+      <c r="F470" s="5">
+        <v>743305600000000</v>
+      </c>
     </row>
     <row r="471" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A471" s="3" t="s">
@@ -10730,6 +10748,12 @@
       <c r="D471" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E471" s="3">
+        <v>2260</v>
+      </c>
+      <c r="F471" s="5">
+        <v>837249500000000</v>
+      </c>
     </row>
     <row r="472" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A472" s="3" t="s">
@@ -10744,6 +10768,15 @@
       <c r="D472" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E472" s="3">
+        <v>4520</v>
+      </c>
+      <c r="F472" s="5">
+        <v>837251000000000</v>
+      </c>
+      <c r="G472" s="9">
+        <v>837251000000000</v>
+      </c>
     </row>
     <row r="473" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A473" s="3" t="s">
@@ -10758,6 +10791,12 @@
       <c r="D473" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E473" s="3">
+        <v>6780</v>
+      </c>
+      <c r="F473" s="5">
+        <v>539233600000000</v>
+      </c>
     </row>
     <row r="474" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A474" s="3" t="s">
@@ -10772,6 +10811,12 @@
       <c r="D474" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E474" s="3">
+        <v>9040.25</v>
+      </c>
+      <c r="F474" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="475" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A475" s="3" t="s">
@@ -10786,6 +10831,12 @@
       <c r="D475" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E475" s="3">
+        <v>0</v>
+      </c>
+      <c r="F475" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="476" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A476" s="3" t="s">
@@ -10800,6 +10851,12 @@
       <c r="D476" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E476" s="3">
+        <v>2260</v>
+      </c>
+      <c r="F476" s="5">
+        <v>418597400000000</v>
+      </c>
     </row>
     <row r="477" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A477" s="3" t="s">
@@ -10814,6 +10871,12 @@
       <c r="D477" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E477" s="3">
+        <v>4520</v>
+      </c>
+      <c r="F477" s="5">
+        <v>418597400000000</v>
+      </c>
     </row>
     <row r="478" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A478" s="3" t="s">
@@ -10828,6 +10891,12 @@
       <c r="D478" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E478" s="3">
+        <v>6780</v>
+      </c>
+      <c r="F478" s="5">
+        <v>269615900000000</v>
+      </c>
     </row>
     <row r="479" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
@@ -10842,6 +10911,12 @@
       <c r="D479" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E479" s="3">
+        <v>9040</v>
+      </c>
+      <c r="F479" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="480" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A480" s="3" t="s">
@@ -10856,8 +10931,14 @@
       <c r="D480" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E480" s="3">
+        <v>-80</v>
+      </c>
+      <c r="F480" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
         <v>17</v>
       </c>
@@ -10870,8 +10951,14 @@
       <c r="D481" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E481" s="3">
+        <v>-45</v>
+      </c>
+      <c r="F481" s="5">
+        <v>236819900000000</v>
+      </c>
+    </row>
+    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A482" s="3" t="s">
         <v>17</v>
       </c>
@@ -10884,8 +10971,14 @@
       <c r="D482" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E482" s="3">
+        <v>-10</v>
+      </c>
+      <c r="F482" s="5">
+        <v>418597400000000</v>
+      </c>
+    </row>
+    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A483" s="3" t="s">
         <v>17</v>
       </c>
@@ -10898,8 +10991,14 @@
       <c r="D483" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E483" s="3">
+        <v>30</v>
+      </c>
+      <c r="F483" s="5">
+        <v>160390000000000</v>
+      </c>
+    </row>
+    <row r="484" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A484" s="3" t="s">
         <v>17</v>
       </c>
@@ -10912,8 +11011,14 @@
       <c r="D484" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E484" s="3">
+        <v>70</v>
+      </c>
+      <c r="F484" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A485" s="3" t="s">
         <v>17</v>
       </c>
@@ -10926,8 +11031,14 @@
       <c r="D485" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E485" s="3">
+        <v>-80</v>
+      </c>
+      <c r="F485" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A486" s="3" t="s">
         <v>17</v>
       </c>
@@ -10940,8 +11051,15 @@
       <c r="D486" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E486" s="3">
+        <v>-45</v>
+      </c>
+      <c r="F486" s="9">
+        <v>473770400000000</v>
+      </c>
+      <c r="G486" s="9"/>
+    </row>
+    <row r="487" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A487" s="3" t="s">
         <v>17</v>
       </c>
@@ -10954,8 +11072,14 @@
       <c r="D487" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E487" s="3">
+        <v>-10</v>
+      </c>
+      <c r="F487" s="5">
+        <v>837251000000000</v>
+      </c>
+    </row>
+    <row r="488" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A488" s="3" t="s">
         <v>17</v>
       </c>
@@ -10968,8 +11092,14 @@
       <c r="D488" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E488" s="3">
+        <v>30</v>
+      </c>
+      <c r="F488" s="5">
+        <v>320876300000000</v>
+      </c>
+    </row>
+    <row r="489" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A489" s="3" t="s">
         <v>17</v>
       </c>
@@ -10982,8 +11112,14 @@
       <c r="D489" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E489" s="3">
+        <v>70</v>
+      </c>
+      <c r="F489" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
         <v>17</v>
       </c>
@@ -10996,8 +11132,14 @@
       <c r="D490" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E490" s="3">
+        <v>-80</v>
+      </c>
+      <c r="F490" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A491" s="3" t="s">
         <v>17</v>
       </c>
@@ -11010,8 +11152,24 @@
       <c r="D491" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E491" s="3">
+        <v>-45</v>
+      </c>
+      <c r="F491" s="3">
+        <v>14016110.35042</v>
+      </c>
+      <c r="G491">
+        <v>15183781.34949</v>
+      </c>
+      <c r="H491">
+        <v>1167670.9990699999</v>
+      </c>
+      <c r="I491">
+        <f>G491-H491</f>
+        <v>14016110.35042</v>
+      </c>
+    </row>
+    <row r="492" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A492" s="3" t="s">
         <v>17</v>
       </c>
@@ -11024,8 +11182,24 @@
       <c r="D492" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E492" s="3">
+        <v>-10</v>
+      </c>
+      <c r="F492" s="3">
+        <v>26051604.789800003</v>
+      </c>
+      <c r="G492">
+        <v>10867823.440300001</v>
+      </c>
+      <c r="H492">
+        <v>15183781.3495</v>
+      </c>
+      <c r="I492">
+        <f>G492+H492</f>
+        <v>26051604.789800003</v>
+      </c>
+    </row>
+    <row r="493" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A493" s="3" t="s">
         <v>17</v>
       </c>
@@ -11038,8 +11212,24 @@
       <c r="D493" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="494" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E493" s="3">
+        <v>30</v>
+      </c>
+      <c r="F493" s="3">
+        <v>11923190.174462002</v>
+      </c>
+      <c r="G493">
+        <v>10867823.440269001</v>
+      </c>
+      <c r="H493">
+        <v>1055366.734193</v>
+      </c>
+      <c r="I493">
+        <f>G493+H493</f>
+        <v>11923190.174462002</v>
+      </c>
+    </row>
+    <row r="494" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A494" s="3" t="s">
         <v>17</v>
       </c>
@@ -11052,8 +11242,14 @@
       <c r="D494" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="495" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E494" s="3">
+        <v>70</v>
+      </c>
+      <c r="F494" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A495" s="3" t="s">
         <v>17</v>
       </c>
@@ -11066,8 +11262,14 @@
       <c r="D495" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="496" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E495" s="3">
+        <v>-178</v>
+      </c>
+      <c r="F495" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
         <v>17</v>
       </c>
@@ -11080,8 +11282,11 @@
       <c r="D496" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E496" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="497" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
         <v>17</v>
       </c>
@@ -11094,8 +11299,14 @@
       <c r="D497" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E497" s="3">
+        <v>0</v>
+      </c>
+      <c r="F497" s="5">
+        <v>418597400000000</v>
+      </c>
+    </row>
+    <row r="498" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
         <v>17</v>
       </c>
@@ -11108,8 +11319,11 @@
       <c r="D498" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E498" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="499" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
         <v>17</v>
       </c>
@@ -11122,8 +11336,14 @@
       <c r="D499" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E499" s="3">
+        <v>178</v>
+      </c>
+      <c r="F499" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
         <v>17</v>
       </c>
@@ -11136,8 +11356,14 @@
       <c r="D500" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E500" s="3">
+        <v>-178</v>
+      </c>
+      <c r="F500" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A501" s="3" t="s">
         <v>17</v>
       </c>
@@ -11150,8 +11376,11 @@
       <c r="D501" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E501" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="502" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A502" s="3" t="s">
         <v>17</v>
       </c>
@@ -11164,8 +11393,14 @@
       <c r="D502" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E502" s="3">
+        <v>0</v>
+      </c>
+      <c r="F502" s="5">
+        <v>837251000000000</v>
+      </c>
+    </row>
+    <row r="503" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A503" s="3" t="s">
         <v>17</v>
       </c>
@@ -11178,8 +11413,11 @@
       <c r="D503" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E503" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="504" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A504" s="3" t="s">
         <v>17</v>
       </c>
@@ -11192,8 +11430,14 @@
       <c r="D504" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E504" s="3">
+        <v>178</v>
+      </c>
+      <c r="F504" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="505" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A505" s="3" t="s">
         <v>17</v>
       </c>
@@ -11206,8 +11450,14 @@
       <c r="D505" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E505" s="3">
+        <v>-178</v>
+      </c>
+      <c r="F505" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="506" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A506" s="3" t="s">
         <v>17</v>
       </c>
@@ -11220,8 +11470,11 @@
       <c r="D506" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E506" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="507" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A507" s="3" t="s">
         <v>17</v>
       </c>
@@ -11234,8 +11487,24 @@
       <c r="D507" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E507" s="3">
+        <v>0</v>
+      </c>
+      <c r="F507" s="3">
+        <v>21039383.760000002</v>
+      </c>
+      <c r="G507">
+        <v>5510314.7943000002</v>
+      </c>
+      <c r="H507">
+        <v>15529068.965700001</v>
+      </c>
+      <c r="I507">
+        <f>G507+H507</f>
+        <v>21039383.760000002</v>
+      </c>
+    </row>
+    <row r="508" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A508" s="3" t="s">
         <v>17</v>
       </c>
@@ -11248,8 +11517,11 @@
       <c r="D508" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E508" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="509" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A509" s="3" t="s">
         <v>17</v>
       </c>
@@ -11262,8 +11534,14 @@
       <c r="D509" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E509" s="3">
+        <v>178</v>
+      </c>
+      <c r="F509" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="510" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A510" s="3" t="s">
         <v>17</v>
       </c>
@@ -11283,7 +11561,7 @@
         <v>17937492727200</v>
       </c>
     </row>
-    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A511" s="3" t="s">
         <v>17</v>
       </c>
@@ -11303,7 +11581,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A512" s="3" t="s">
         <v>17</v>
       </c>
@@ -12497,7 +12775,7 @@
         <v>5207596530660</v>
       </c>
       <c r="I563">
-        <f t="shared" ref="I563:I565" si="6">G563-H563</f>
+        <f t="shared" ref="I563:I564" si="6">G563-H563</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>